<commit_message>
Added Repo, more attribute, database mapping
</commit_message>
<xml_diff>
--- a/buytandoors_design/Book 1.xlsx
+++ b/buytandoors_design/Book 1.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="139">
   <si>
     <t xml:space="preserve">Features </t>
   </si>
@@ -79,9 +79,6 @@
     <t>Electric</t>
   </si>
   <si>
-    <t xml:space="preserve">Stainless Steel </t>
-  </si>
-  <si>
     <t>Mild Steel</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
   </si>
   <si>
     <t>Includes</t>
-  </si>
-  <si>
-    <t>GENERAL</t>
   </si>
   <si>
     <t xml:space="preserve">Body Material </t>
@@ -345,6 +339,114 @@
   </si>
   <si>
     <t>Option 8</t>
+  </si>
+  <si>
+    <t>Option 9</t>
+  </si>
+  <si>
+    <t>Option 10</t>
+  </si>
+  <si>
+    <t>Option 11</t>
+  </si>
+  <si>
+    <t>Home Extra Small</t>
+  </si>
+  <si>
+    <t>Home Small</t>
+  </si>
+  <si>
+    <t>Home X Extra Small</t>
+  </si>
+  <si>
+    <t>Stainless Steel</t>
+  </si>
+  <si>
+    <t>Barrel</t>
+  </si>
+  <si>
+    <t>Table1</t>
+  </si>
+  <si>
+    <t>SizeID</t>
+  </si>
+  <si>
+    <t>ShapeID</t>
+  </si>
+  <si>
+    <t>Table2</t>
+  </si>
+  <si>
+    <t>ProductId</t>
+  </si>
+  <si>
+    <t>Table3</t>
+  </si>
+  <si>
+    <t>ShapeId</t>
+  </si>
+  <si>
+    <t>Table4</t>
+  </si>
+  <si>
+    <t>WeightID</t>
+  </si>
+  <si>
+    <t>Table5</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Baral</t>
+  </si>
+  <si>
+    <t>Table6</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>WeightId</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Tandoors</t>
+  </si>
+  <si>
+    <t>Pizza Oven</t>
+  </si>
+  <si>
+    <t>Catering</t>
+  </si>
+  <si>
+    <t>MS Body</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Wall Fitting</t>
+  </si>
+  <si>
+    <t>Barbeque</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>Wood Fire</t>
+  </si>
+  <si>
+    <t>Gas Fire</t>
+  </si>
+  <si>
+    <t>Hybrid Fire</t>
   </si>
 </sst>
 </file>
@@ -435,9 +537,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I28" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:I28"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L29" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:L29"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="Features "/>
     <tableColumn id="2" name="Options 1"/>
     <tableColumn id="3" name="Option 2"/>
@@ -447,6 +549,9 @@
     <tableColumn id="7" name="Option 6"/>
     <tableColumn id="8" name="Option 7"/>
     <tableColumn id="9" name="Option 8"/>
+    <tableColumn id="10" name="Option 9"/>
+    <tableColumn id="11" name="Option 10"/>
+    <tableColumn id="12" name="Option 11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -749,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,9 +869,10 @@
     <col min="5" max="5" width="18.109375" customWidth="1"/>
     <col min="6" max="7" width="18.44140625" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,12 +898,21 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -809,21 +924,21 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
@@ -839,57 +954,59 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -910,163 +1027,217 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="K8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="I12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="H13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="B14" s="1">
         <v>4</v>
@@ -1079,12 +1250,12 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1096,37 +1267,37 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1136,35 +1307,35 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="C18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1174,9 +1345,9 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1187,62 +1358,62 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
         <v>63</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>64</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>65</v>
       </c>
-      <c r="D21" t="s">
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B22" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="B23" t="s">
         <v>69</v>
       </c>
-      <c r="B23" t="s">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="B24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1252,15 +1423,15 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1268,26 +1439,292 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
         <v>98</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G28" t="s">
+        <v>110</v>
+      </c>
+      <c r="H28" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J28" t="s">
+        <v>134</v>
+      </c>
+      <c r="K28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43">
         <v>100</v>
       </c>
-      <c r="D27" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
product structure with repository
</commit_message>
<xml_diff>
--- a/buytandoors_design/Book 1.xlsx
+++ b/buytandoors_design/Book 1.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14388" yWindow="-12" windowWidth="14436" windowHeight="12840"/>
+    <workbookView xWindow="14388" yWindow="-12" windowWidth="14436" windowHeight="12840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="140">
   <si>
     <t xml:space="preserve">Features </t>
   </si>
@@ -447,6 +448,9 @@
   </si>
   <si>
     <t>Hybrid Fire</t>
+  </si>
+  <si>
+    <t>Clay Tandoor</t>
   </si>
 </sst>
 </file>
@@ -854,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1292,7 +1296,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
@@ -1307,7 +1311,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>54</v>
       </c>
@@ -1330,7 +1334,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>56</v>
       </c>
@@ -1345,7 +1349,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>60</v>
       </c>
@@ -1358,7 +1362,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -1373,7 +1377,7 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
@@ -1382,7 +1386,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
@@ -1391,7 +1395,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -1411,7 +1415,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -1423,7 +1427,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>88</v>
       </c>
@@ -1439,7 +1443,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>75</v>
       </c>
@@ -1454,7 +1458,7 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>126</v>
       </c>
@@ -1488,8 +1492,11 @@
       <c r="K28" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>129</v>
       </c>
@@ -1504,226 +1511,6 @@
       </c>
       <c r="G29" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>2</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>2</v>
-      </c>
-      <c r="B34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>3</v>
-      </c>
-      <c r="B42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>4</v>
-      </c>
-      <c r="B43" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>2</v>
-      </c>
-      <c r="B44" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>2</v>
-      </c>
-      <c r="B45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>119</v>
-      </c>
-      <c r="B47" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>4</v>
-      </c>
-      <c r="B48">
-        <v>3</v>
-      </c>
-      <c r="C48">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C49">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C50">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>124</v>
-      </c>
-      <c r="B57" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" t="s">
-        <v>113</v>
-      </c>
-      <c r="D57" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58">
-        <v>2</v>
-      </c>
-      <c r="D58">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>1</v>
-      </c>
-      <c r="B59">
-        <v>2</v>
-      </c>
-      <c r="C59">
-        <v>2</v>
-      </c>
-      <c r="D59">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>1</v>
-      </c>
-      <c r="B60">
-        <v>3</v>
-      </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
-      <c r="D60">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1733,4 +1520,326 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" t="s">
+        <v>113</v>
+      </c>
+      <c r="J4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>34</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
size & repository work.
</commit_message>
<xml_diff>
--- a/buytandoors_design/Book 1.xlsx
+++ b/buytandoors_design/Book 1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14388" yWindow="-12" windowWidth="14436" windowHeight="12840" activeTab="1"/>
+    <workbookView xWindow="14388" yWindow="-12" windowWidth="14436" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="144">
   <si>
     <t xml:space="preserve">Features </t>
   </si>
@@ -242,9 +242,6 @@
     <t>Wooden Crate</t>
   </si>
   <si>
-    <t>Gross Weight</t>
-  </si>
-  <si>
     <t>Net Weight</t>
   </si>
   <si>
@@ -264,21 +261,6 @@
   </si>
   <si>
     <t>ISO</t>
-  </si>
-  <si>
-    <t>10 to 12</t>
-  </si>
-  <si>
-    <t>15 to 18</t>
-  </si>
-  <si>
-    <t>20 to 22</t>
-  </si>
-  <si>
-    <t>24 to 25</t>
-  </si>
-  <si>
-    <t>28 to 30</t>
   </si>
   <si>
     <t>30+</t>
@@ -451,6 +433,36 @@
   </si>
   <si>
     <t>Clay Tandoor</t>
+  </si>
+  <si>
+    <t>5 to 8</t>
+  </si>
+  <si>
+    <t>8 to 10</t>
+  </si>
+  <si>
+    <t>11 to 12</t>
+  </si>
+  <si>
+    <t>13 to 15</t>
+  </si>
+  <si>
+    <t>16 to 18</t>
+  </si>
+  <si>
+    <t>19 to 20</t>
+  </si>
+  <si>
+    <t>21 to 25</t>
+  </si>
+  <si>
+    <t>26 to 28</t>
+  </si>
+  <si>
+    <t>Gross Weight square</t>
+  </si>
+  <si>
+    <t>Gross Weight Brass</t>
   </si>
 </sst>
 </file>
@@ -541,8 +553,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L29" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:L29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L30" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:L30"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Features "/>
     <tableColumn id="2" name="Options 1"/>
@@ -858,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,16 +914,16 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -928,13 +940,13 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>11</v>
@@ -960,10 +972,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
@@ -990,7 +1002,7 @@
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>11</v>
@@ -1036,13 +1048,13 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>26</v>
@@ -1069,38 +1081,38 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1276,32 +1288,39 @@
         <v>52</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>79</v>
+        <v>135</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+        <v>139</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J16" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1319,16 +1338,16 @@
         <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1397,119 +1416,135 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" t="s">
-        <v>93</v>
+        <v>142</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>60</v>
+      </c>
+      <c r="D24">
+        <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="G24" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" t="s">
+        <v>88</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+        <v>143</v>
+      </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" t="s">
-        <v>97</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B28" t="s">
+      <c r="G29" t="s">
+        <v>104</v>
+      </c>
+      <c r="H29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" t="s">
         <v>127</v>
       </c>
-      <c r="C28" t="s">
+      <c r="J29" t="s">
         <v>128</v>
       </c>
-      <c r="D28" t="s">
+      <c r="K29" t="s">
+        <v>129</v>
+      </c>
+      <c r="L29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E30" t="s">
         <v>131</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G28" t="s">
-        <v>110</v>
-      </c>
-      <c r="H28" t="s">
-        <v>74</v>
-      </c>
-      <c r="I28" t="s">
-        <v>133</v>
-      </c>
-      <c r="J28" t="s">
-        <v>134</v>
-      </c>
-      <c r="K28" t="s">
-        <v>135</v>
-      </c>
-      <c r="L28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>129</v>
-      </c>
-      <c r="D29" t="s">
-        <v>136</v>
-      </c>
-      <c r="E29" t="s">
-        <v>137</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="G30" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1526,44 +1561,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
@@ -1671,18 +1706,18 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
@@ -1712,7 +1747,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D16">
         <v>150</v>
@@ -1728,18 +1763,18 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
@@ -1765,12 +1800,12 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
@@ -1780,21 +1815,21 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E29" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
all fix & product weight logic
</commit_message>
<xml_diff>
--- a/buytandoors_design/Book 1.xlsx
+++ b/buytandoors_design/Book 1.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="150">
   <si>
     <t xml:space="preserve">Features </t>
   </si>
@@ -472,6 +472,15 @@
   </si>
   <si>
     <t>Poly</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Gaudge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to </t>
   </si>
 </sst>
 </file>
@@ -562,8 +571,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L31" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:L31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L33" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:L33"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Features "/>
     <tableColumn id="2" name="Options 1"/>
@@ -879,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1568,6 +1577,33 @@
         <v>146</v>
       </c>
       <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32">
+        <v>202</v>
+      </c>
+      <c r="C32">
+        <v>304</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33">
+        <v>18</v>
+      </c>
+      <c r="F33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>